<commit_message>
support for None to avoid entering values into an Excel input range
</commit_message>
<xml_diff>
--- a/test/test_book.xlsx
+++ b/test/test_book.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rteachey\projects\excalc\test\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4BB4BBB-5E40-488D-ABD2-5EB06D2ED208}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{305BB3A0-6B15-4437-BF75-20DC5161736C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{510CAF83-A846-41F0-A6ED-23821BDED279}"/>
   </bookViews>
@@ -403,7 +403,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{315C5C03-1E21-41E0-8CBB-C260289CB421}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>

</xml_diff>